<commit_message>
Use large instances instead of medium instances.
</commit_message>
<xml_diff>
--- a/projects/case2012_seb_report.xlsx
+++ b/projects/case2012_seb_report.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\OpenStudio-fault-models\projects\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="29040" windowHeight="15990" tabRatio="562"/>
   </bookViews>
@@ -30,7 +35,7 @@
     <definedName name="TrueFalse">Lookups!$C$14:$C$15</definedName>
     <definedName name="Workflow">Lookups!$E$14:$E$15</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -2923,7 +2928,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="27" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -6731,6 +6736,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -6778,7 +6786,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -6813,7 +6821,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -7025,7 +7033,7 @@
   <dimension ref="A1:F51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7107,19 +7115,19 @@
         <v>441</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>637</v>
+        <v>590</v>
       </c>
       <c r="C7" s="24" t="str">
         <f>VLOOKUP($B7,instance_defs,5,FALSE)</f>
-        <v>Use only for cluster configuration testing</v>
+        <v>Recommended for Server</v>
       </c>
       <c r="D7" s="24" t="str">
         <f>VLOOKUP($B7,instance_defs,2,FALSE)&amp;" with "&amp;VLOOKUP($B7,instance_defs,4,FALSE)</f>
-        <v>1 Cores with 4 GB</v>
+        <v>2 Cores with 32 GB</v>
       </c>
       <c r="E7" s="24" t="str">
         <f>VLOOKUP($B7,instance_defs,3,FALSE)</f>
-        <v>$0.07/hour</v>
+        <v>$0.14/hour</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>605</v>
@@ -7161,7 +7169,7 @@
       </c>
       <c r="E9" s="24" t="str">
         <f>"$"&amp;VALUE(LEFT(E7,5))+B9*VALUE(LEFT(E8,5))&amp;"/hour"</f>
-        <v>$0.21/hour</v>
+        <v>$0.28/hour</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>707</v>

</xml_diff>